<commit_message>
Caricamento report 01/04/2022 Signorbet
</commit_message>
<xml_diff>
--- a/2022_04.xlsx
+++ b/2022_04.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ReportScommesse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6E2E53-897B-473C-87C8-740417C8221F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1897B5B1-9B35-4D20-9F7C-F42A71AEE55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{51CCC196-2655-4572-B028-F9E61E569708}"/>
+    <workbookView xWindow="10725" yWindow="825" windowWidth="17985" windowHeight="19065" xr2:uid="{51CCC196-2655-4572-B028-F9E61E569708}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>DATA</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>BASKET</t>
+  </si>
+  <si>
+    <t>PERSA</t>
   </si>
 </sst>
 </file>
@@ -140,7 +143,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,6 +153,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -379,18 +388,6 @@
     <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -409,18 +406,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -744,23 +760,23 @@
   <dimension ref="B1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="6.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="6.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
@@ -771,25 +787,25 @@
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="33"/>
+      <c r="G2" s="29"/>
       <c r="H2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="33"/>
+      <c r="K2" s="29"/>
       <c r="L2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="13">
         <v>19.5</v>
       </c>
@@ -800,42 +816,48 @@
       <c r="E3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="36"/>
-      <c r="G3" s="37"/>
+      <c r="F3" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="39"/>
       <c r="H3" s="11">
         <v>-15</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="34">
+      <c r="I3" s="40"/>
+      <c r="J3" s="32">
         <f>B3+(I3+H3)</f>
         <v>4.5</v>
       </c>
-      <c r="K3" s="35"/>
+      <c r="K3" s="33"/>
       <c r="L3" s="17">
         <f>I3+H3</f>
         <v>-15</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="6">
         <v>44652</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="11"/>
+      <c r="E4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="30"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="11">
+        <v>-4</v>
+      </c>
       <c r="I4" s="23"/>
-      <c r="J4" s="28">
+      <c r="J4" s="24">
         <f>J3+(I4+H4)</f>
-        <v>4.5</v>
-      </c>
-      <c r="K4" s="29"/>
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="25"/>
       <c r="L4" s="16">
         <f>I4+H4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -844,488 +866,488 @@
         <v>44653</v>
       </c>
       <c r="E5" s="12"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="37"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="31"/>
       <c r="H5" s="22"/>
       <c r="I5" s="23"/>
-      <c r="J5" s="28">
+      <c r="J5" s="24">
         <f t="shared" ref="J5:J31" si="0">J4+(I5+H5)</f>
-        <v>4.5</v>
-      </c>
-      <c r="K5" s="29"/>
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="25"/>
       <c r="L5" s="16">
         <f t="shared" ref="L5:L31" si="1">I5+H5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="13">
         <f>B3+L32</f>
-        <v>4.5</v>
+        <v>0.5</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="6">
         <v>44654</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="31"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="22"/>
       <c r="I6" s="21"/>
-      <c r="J6" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K6" s="29"/>
+      <c r="J6" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="25"/>
       <c r="L6" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="6">
         <v>44655</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="31"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="22"/>
       <c r="I7" s="23"/>
-      <c r="J7" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K7" s="29"/>
+      <c r="J7" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="25"/>
       <c r="L7" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="6"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="31"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="22"/>
       <c r="I8" s="21"/>
-      <c r="J8" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K8" s="29"/>
+      <c r="J8" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="25"/>
       <c r="L8" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="13">
         <f>B6-B3</f>
-        <v>-15</v>
+        <v>-19</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="6"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="31"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="22"/>
       <c r="I9" s="21"/>
-      <c r="J9" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K9" s="29"/>
+      <c r="J9" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="25"/>
       <c r="L9" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="6"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="31"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="22"/>
       <c r="I10" s="21"/>
-      <c r="J10" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K10" s="29"/>
+      <c r="J10" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="25"/>
       <c r="L10" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="31"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="22"/>
       <c r="I11" s="21"/>
-      <c r="J11" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K11" s="29"/>
+      <c r="J11" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="25"/>
       <c r="L11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="13">
         <f>MAX(J3:K31)-B3</f>
         <v>-15</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="31"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="22"/>
       <c r="I12" s="23"/>
-      <c r="J12" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K12" s="29"/>
+      <c r="J12" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K12" s="25"/>
       <c r="L12" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D13" s="6"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="31"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="22"/>
       <c r="I13" s="21"/>
-      <c r="J13" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K13" s="29"/>
+      <c r="J13" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K13" s="25"/>
       <c r="L13" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D14" s="6"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="31"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="27"/>
       <c r="H14" s="22"/>
       <c r="I14" s="21"/>
-      <c r="J14" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K14" s="29"/>
+      <c r="J14" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K14" s="25"/>
       <c r="L14" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D15" s="6"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27"/>
       <c r="H15" s="22"/>
       <c r="I15" s="21"/>
-      <c r="J15" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K15" s="29"/>
+      <c r="J15" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K15" s="25"/>
       <c r="L15" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D16" s="6"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="31"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="27"/>
       <c r="H16" s="22"/>
       <c r="I16" s="21"/>
-      <c r="J16" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K16" s="29"/>
+      <c r="J16" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K16" s="25"/>
       <c r="L16" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D17" s="6"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="31"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="22"/>
       <c r="I17" s="21"/>
-      <c r="J17" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K17" s="29"/>
+      <c r="J17" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K17" s="25"/>
       <c r="L17" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D18" s="6"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="27"/>
       <c r="H18" s="22"/>
       <c r="I18" s="21"/>
-      <c r="J18" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K18" s="29"/>
+      <c r="J18" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K18" s="25"/>
       <c r="L18" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D19" s="6"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="31"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="27"/>
       <c r="H19" s="22"/>
       <c r="I19" s="21"/>
-      <c r="J19" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K19" s="29"/>
+      <c r="J19" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K19" s="25"/>
       <c r="L19" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D20" s="6"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="31"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
       <c r="H20" s="22"/>
       <c r="I20" s="21"/>
-      <c r="J20" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K20" s="29"/>
+      <c r="J20" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K20" s="25"/>
       <c r="L20" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D21" s="6"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="31"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="27"/>
       <c r="H21" s="22"/>
       <c r="I21" s="21"/>
-      <c r="J21" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K21" s="29"/>
+      <c r="J21" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K21" s="25"/>
       <c r="L21" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D22" s="6"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="31"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="27"/>
       <c r="H22" s="22"/>
       <c r="I22" s="21"/>
-      <c r="J22" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K22" s="29"/>
+      <c r="J22" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K22" s="25"/>
       <c r="L22" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D23" s="6"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="31"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="22"/>
       <c r="I23" s="21"/>
-      <c r="J23" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K23" s="29"/>
+      <c r="J23" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K23" s="25"/>
       <c r="L23" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D24" s="6"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="31"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
       <c r="H24" s="22"/>
       <c r="I24" s="21"/>
-      <c r="J24" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K24" s="29"/>
+      <c r="J24" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K24" s="25"/>
       <c r="L24" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D25" s="6"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="31"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="27"/>
       <c r="H25" s="22"/>
       <c r="I25" s="21"/>
-      <c r="J25" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K25" s="29"/>
+      <c r="J25" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K25" s="25"/>
       <c r="L25" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D26" s="6"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="31"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="27"/>
       <c r="H26" s="22"/>
       <c r="I26" s="21"/>
-      <c r="J26" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K26" s="29"/>
+      <c r="J26" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K26" s="25"/>
       <c r="L26" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D27" s="6"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="31"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="27"/>
       <c r="H27" s="22"/>
       <c r="I27" s="21"/>
-      <c r="J27" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K27" s="29"/>
+      <c r="J27" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K27" s="25"/>
       <c r="L27" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D28" s="6"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
       <c r="H28" s="22"/>
       <c r="I28" s="21"/>
-      <c r="J28" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K28" s="29"/>
+      <c r="J28" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K28" s="25"/>
       <c r="L28" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D29" s="6"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="31"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="27"/>
       <c r="H29" s="22"/>
       <c r="I29" s="21"/>
-      <c r="J29" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K29" s="29"/>
+      <c r="J29" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K29" s="25"/>
       <c r="L29" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D30" s="6"/>
       <c r="E30" s="4"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="31"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="27"/>
       <c r="H30" s="22"/>
       <c r="I30" s="21"/>
-      <c r="J30" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K30" s="29"/>
+      <c r="J30" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K30" s="25"/>
       <c r="L30" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="6"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
       <c r="H31" s="22"/>
       <c r="I31" s="21"/>
-      <c r="J31" s="28">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K31" s="29"/>
+      <c r="J31" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K31" s="25"/>
       <c r="L31" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="8">
         <v>44652</v>
       </c>
@@ -1336,78 +1358,32 @@
       </c>
       <c r="G32" s="2">
         <f>COUNTIF(F3:G31,"PERSA")+COUNTIF(F3:G31,"VINTA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="13">
         <f>SUM(H3:H31)</f>
-        <v>-15</v>
+        <v>-19</v>
       </c>
       <c r="I32" s="15">
         <f>SUM(I3:I31)</f>
         <v>0</v>
       </c>
-      <c r="J32" s="26"/>
-      <c r="K32" s="27"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="37"/>
       <c r="L32" s="14">
         <f>SUM(L3:L31)</f>
-        <v>-15</v>
-      </c>
-    </row>
-    <row r="33" spans="6:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F33" s="24" t="e">
+        <v>-19</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F33" s="34">
         <f>F32/G32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G33" s="25"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
     <mergeCell ref="F33:G33"/>
     <mergeCell ref="J32:K32"/>
     <mergeCell ref="J22:K22"/>
@@ -1424,6 +1400,52 @@
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="F11:G11"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J30:K30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>